<commit_message>
Docs files and other.
</commit_message>
<xml_diff>
--- a/docs/BasicPostProcess_flask.xlsx
+++ b/docs/BasicPostProcess_flask.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="BLEUScore" sheetId="1" r:id="rId1"/>
-    <sheet name="CompilationAndTestsRan" sheetId="2" r:id="rId2"/>
+    <sheet name="BLEUBasic" sheetId="1" r:id="rId1"/>
+    <sheet name="CompilationBasic" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="bleu_score_evaluation" localSheetId="0">BLEUScore!$A$1:$C$170</definedName>
-    <definedName name="compiler_evaluation" localSheetId="1">CompilationAndTestsRan!$A$1:$D$96</definedName>
+    <definedName name="bleu_score_evaluation" localSheetId="0">BLEUBasic!$A$1:$C$170</definedName>
+    <definedName name="compiler_evaluation" localSheetId="1">CompilationBasic!$A$1:$D$96</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1111,17 +1111,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C170"/>
+  <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2990,6 +2990,12 @@
       </c>
       <c r="C170" s="2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="3">
+        <f>SUM(C2:C170)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3002,9 +3008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
-    </sheetView>
+    <sheetView topLeftCell="A76" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>